<commit_message>
Leccion 9 excel y tablas de datos
</commit_message>
<xml_diff>
--- a/Archivos para practicas/challenge.xlsx
+++ b/Archivos para practicas/challenge.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amontilla\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amontilla\Documents\UiPath\Intro\Archivos para practicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F93611A-4390-4594-91D5-04CDF0671E29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C229DFCB-D24B-4608-BADB-D188583C46C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Dorsey</t>
   </si>
   <si>
-    <t>MediCare</t>
-  </si>
-  <si>
     <t>Medical Engineer</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
   </si>
   <si>
     <t>IT Specialist</t>
-  </si>
-  <si>
-    <t>17 Farburn Terrace</t>
   </si>
   <si>
     <t>Doug</t>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>Last Name</t>
+  </si>
+  <si>
+    <t>MediCare1</t>
+  </si>
+  <si>
+    <t>MediCare123</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -675,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="4">
         <v>40716543298</v>
@@ -690,16 +690,16 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="4">
         <v>40791345621</v>
@@ -708,22 +708,22 @@
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4">
         <v>40735416854</v>
@@ -732,22 +732,22 @@
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="4">
         <v>40733652145</v>
@@ -756,22 +756,22 @@
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="4">
         <v>40799885412</v>
@@ -780,22 +780,22 @@
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G7" s="4">
         <v>40733154268</v>
@@ -804,22 +804,22 @@
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G8" s="4">
         <v>40712462257</v>
@@ -828,22 +828,22 @@
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G9" s="4">
         <v>40731254562</v>
@@ -852,22 +852,22 @@
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4">
         <v>40741785214</v>
@@ -876,22 +876,22 @@
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4">
         <v>40731653845</v>
@@ -10808,7 +10808,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -10843,7 +10843,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="4">
         <v>40716543298</v>

</xml_diff>